<commit_message>
Added HW resources info to pinout spreadsheet
</commit_message>
<xml_diff>
--- a/extpins.xlsx
+++ b/extpins.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\roman\robot-yandex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romankh\home\yabot\yagit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,227 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+  <si>
+    <t>SCH signal</t>
+  </si>
+  <si>
+    <t>SCH N</t>
+  </si>
+  <si>
+    <t>Jetson Socket N</t>
+  </si>
+  <si>
+    <t>DevKit Signal</t>
+  </si>
+  <si>
+    <t>SOC signal</t>
+  </si>
+  <si>
+    <t>AUDIO_I2S_MCLK_3V3</t>
+  </si>
+  <si>
+    <t>AUDIO_MCLK</t>
+  </si>
+  <si>
+    <t>Real HW</t>
+  </si>
+  <si>
+    <t>AUDIO_I2S_SRCLK_3V3</t>
+  </si>
+  <si>
+    <t>I2S0_SCLK</t>
+  </si>
+  <si>
+    <t>AUDIO_CDC_IRQ_LVL</t>
+  </si>
+  <si>
+    <t>MDM_WAKE_AP_LVL</t>
+  </si>
+  <si>
+    <t>GPIO20</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>SPI1_MOSI_3V3</t>
+  </si>
+  <si>
+    <t>SPI1_MOSI</t>
+  </si>
+  <si>
+    <t>SPI1_MISO_3V3</t>
+  </si>
+  <si>
+    <t>SPI1_MISO</t>
+  </si>
+  <si>
+    <t>SPI1_SCK_3V3</t>
+  </si>
+  <si>
+    <t>SPI1_CLK</t>
+  </si>
+  <si>
+    <t>SPI1_CS0_3V3</t>
+  </si>
+  <si>
+    <t>SPI1_CS0#</t>
+  </si>
+  <si>
+    <t>I2C_GP1_DAT_3V3</t>
+  </si>
+  <si>
+    <t>I2C_GP1_DAT</t>
+  </si>
+  <si>
+    <t>I2C_GP1_CLK_3V3</t>
+  </si>
+  <si>
+    <t>I2C_GP1_CLK</t>
+  </si>
+  <si>
+    <t>AUD_RST_LVL</t>
+  </si>
+  <si>
+    <t>GPIO19</t>
+  </si>
+  <si>
+    <t>MOTION_INT_AP_L_LVL</t>
+  </si>
+  <si>
+    <t>GPIO9</t>
+  </si>
+  <si>
+    <t>AP_WAKE_BT_3V3</t>
+  </si>
+  <si>
+    <t>GPIO11</t>
+  </si>
+  <si>
+    <t>AUDIO_I2S_SFSYNC_3V3</t>
+  </si>
+  <si>
+    <t>I2S0_LRCLK</t>
+  </si>
+  <si>
+    <t>SAR_TOUT_LVL</t>
+  </si>
+  <si>
+    <t>GPIO8</t>
+  </si>
+  <si>
+    <t>AUDIO_I2S_SIN_3V3</t>
+  </si>
+  <si>
+    <t>I2S0_SDIN</t>
+  </si>
+  <si>
+    <t>AUDIO_I2S_SOUT_3V3</t>
+  </si>
+  <si>
+    <t>I2S0_SDOUT</t>
+  </si>
+  <si>
+    <t>I2S1_CLK</t>
+  </si>
+  <si>
+    <t>I2S1_SDOUT</t>
+  </si>
+  <si>
+    <t>I2S1_SDIN</t>
+  </si>
+  <si>
+    <t>I2S1_LRCLK</t>
+  </si>
+  <si>
+    <t>I2S_SCLK</t>
+  </si>
+  <si>
+    <t>O20</t>
+  </si>
+  <si>
+    <t>O16</t>
+  </si>
+  <si>
+    <t>O19</t>
+  </si>
+  <si>
+    <t>O9</t>
+  </si>
+  <si>
+    <t>O11</t>
+  </si>
+  <si>
+    <t>O8</t>
+  </si>
+  <si>
+    <t>SPI_MOSI</t>
+  </si>
+  <si>
+    <t>SPI_MISO</t>
+  </si>
+  <si>
+    <t>SPI_CLK</t>
+  </si>
+  <si>
+    <t>SPI_CS</t>
+  </si>
+  <si>
+    <t>I2C_SDA</t>
+  </si>
+  <si>
+    <t>I2C_SCL</t>
+  </si>
+  <si>
+    <t>I2S_LRCLK</t>
+  </si>
+  <si>
+    <t>I2S_SDIN</t>
+  </si>
+  <si>
+    <t>I2S_SDOUT</t>
+  </si>
+  <si>
+    <t>I2S-2</t>
+  </si>
+  <si>
+    <t>I2S-1</t>
+  </si>
+  <si>
+    <t>AUD_MCLK</t>
+  </si>
+  <si>
+    <t>SPI-4</t>
+  </si>
+  <si>
+    <t>I2C-1</t>
+  </si>
+  <si>
+    <t>GPIO3_PJ.05</t>
+  </si>
+  <si>
+    <t>GPIO3_PY.01</t>
+  </si>
+  <si>
+    <t>GPIO3_PJ.06</t>
+  </si>
+  <si>
+    <t>GPIO3_PAA.02</t>
+  </si>
+  <si>
+    <t>GPIO3_PI.05</t>
+  </si>
+  <si>
+    <t>GPIO3_PI.04</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,6 +255,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -179,6 +414,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,22 +740,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -523,8 +774,26 @@
         <f>C1+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -538,8 +807,26 @@
         <f t="shared" ref="F2:F20" si="1">C2+1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9">
+        <v>7</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -553,8 +840,26 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="9">
+        <v>2</v>
+      </c>
+      <c r="J3" s="9">
+        <v>12</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>4</v>
       </c>
@@ -570,8 +875,26 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="9">
+        <v>3</v>
+      </c>
+      <c r="J4" s="9">
+        <v>13</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -585,8 +908,26 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="9">
+        <v>4</v>
+      </c>
+      <c r="J5" s="9">
+        <v>18</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>6</v>
       </c>
@@ -602,8 +943,26 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9">
+        <v>19</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>7</v>
       </c>
@@ -619,8 +978,24 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="9">
+        <v>6</v>
+      </c>
+      <c r="J7" s="9">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>8</v>
       </c>
@@ -634,8 +1009,24 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="9">
+        <v>7</v>
+      </c>
+      <c r="J8" s="9">
+        <v>23</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9</v>
       </c>
@@ -651,8 +1042,24 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="9">
+        <v>8</v>
+      </c>
+      <c r="J9" s="9">
+        <v>24</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>10</v>
       </c>
@@ -668,8 +1075,26 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="9">
+        <v>9</v>
+      </c>
+      <c r="J10" s="9">
+        <v>27</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>11</v>
       </c>
@@ -685,8 +1110,24 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="9">
+        <v>10</v>
+      </c>
+      <c r="J11" s="9">
+        <v>28</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>12</v>
       </c>
@@ -704,8 +1145,26 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="9">
+        <v>11</v>
+      </c>
+      <c r="J12" s="9">
+        <v>29</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>13</v>
       </c>
@@ -719,8 +1178,26 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="9">
+        <v>12</v>
+      </c>
+      <c r="J13" s="9">
+        <v>31</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>14</v>
       </c>
@@ -738,8 +1215,26 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="9">
+        <v>13</v>
+      </c>
+      <c r="J14" s="9">
+        <v>33</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>15</v>
       </c>
@@ -755,8 +1250,26 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="9">
+        <v>14</v>
+      </c>
+      <c r="J15" s="9">
+        <v>35</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>16</v>
       </c>
@@ -772,8 +1285,26 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="9">
+        <v>15</v>
+      </c>
+      <c r="J16" s="9">
+        <v>37</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>17</v>
       </c>
@@ -789,8 +1320,26 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="9">
+        <v>16</v>
+      </c>
+      <c r="J17" s="9">
+        <v>38</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>18</v>
       </c>
@@ -806,8 +1355,24 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="9">
+        <v>17</v>
+      </c>
+      <c r="J18" s="9">
+        <v>40</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>19</v>
       </c>
@@ -826,7 +1391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>20</v>
       </c>
@@ -843,8 +1408,64 @@
         <v>40</v>
       </c>
     </row>
+    <row r="23" spans="1:13" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>24</v>
+      </c>
+      <c r="K24" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="13"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" t="s">
+        <v>42</v>
+      </c>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>26</v>
+      </c>
+      <c r="K26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="13"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M6:M9"/>
+    <mergeCell ref="M10:M11"/>
+  </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="200" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="200" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>